<commit_message>
added more formatting to auto reporting, added plot to auto report
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Gain Testing Report</t>
   </si>
@@ -22,10 +22,16 @@
     <t>Date:</t>
   </si>
   <si>
+    <t>DUT Label:</t>
+  </si>
+  <si>
     <t>Customer:</t>
   </si>
   <si>
     <t>NGRF Internal</t>
+  </si>
+  <si>
+    <t>DUT Serial Number:</t>
   </si>
   <si>
     <t>Tested By:</t>
@@ -245,6 +251,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="17487900" cy="8553450"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="2" name="Image 2"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -547,7 +578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,77 +597,85 @@
     <col customWidth="1" max="10" min="10" width="20"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50" r="1" spans="1:10">
+    <row customHeight="1" ht="50" r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>42928</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s"/>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J7" s="6" t="n">
         <v>100000000</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6">
         <f>MAX(B11:B111)</f>
@@ -663,15 +702,15 @@
         <v/>
       </c>
       <c r="I8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J8" s="6" t="n">
         <v>200000</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6">
         <f>AVERAGE(B11:B111)</f>
@@ -698,42 +737,42 @@
         <v/>
       </c>
       <c r="I9" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J10" s="6" t="n">
         <v>0.025</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="6" t="n">
         <v>0</v>
       </c>
@@ -756,10 +795,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="6" t="n">
         <v>3.6</v>
       </c>
@@ -782,13 +821,13 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J12" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="6" t="n">
         <v>7.2</v>
       </c>
@@ -811,13 +850,13 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J13" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="6" t="n">
         <v>10.8</v>
       </c>
@@ -840,13 +879,13 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J14" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="6" t="n">
         <v>14.4</v>
       </c>
@@ -869,13 +908,13 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="6" t="n">
         <v>18</v>
       </c>
@@ -898,13 +937,13 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J16" s="6" t="n">
         <v>-21.99020831627661</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="6" t="n">
         <v>21.6</v>
       </c>
@@ -927,13 +966,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J17" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" s="6" t="n">
         <v>25.2</v>
       </c>
@@ -956,13 +995,13 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J18" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" s="6" t="n">
         <v>28.8</v>
       </c>
@@ -985,13 +1024,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J19" s="6" t="n">
         <v>-21.99020831627661</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" s="6" t="n">
         <v>32.4</v>
       </c>
@@ -1014,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" s="6" t="n">
         <v>36</v>
       </c>
@@ -1037,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22" s="6" t="n">
         <v>39.6</v>
       </c>
@@ -1060,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="A23" s="6" t="n">
         <v>43.2</v>
       </c>
@@ -1083,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="A24" s="6" t="n">
         <v>46.8</v>
       </c>
@@ -1106,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="A25" s="6" t="n">
         <v>50.4</v>
       </c>
@@ -1129,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="A26" s="6" t="n">
         <v>54</v>
       </c>
@@ -1152,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" s="6" t="n">
         <v>57.6</v>
       </c>
@@ -1175,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="A28" s="6" t="n">
         <v>61.2</v>
       </c>
@@ -1198,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29" s="6" t="n">
         <v>64.8</v>
       </c>
@@ -1221,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:11">
       <c r="A30" s="6" t="n">
         <v>68.40000000000001</v>
       </c>
@@ -1244,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31" s="6" t="n">
         <v>72</v>
       </c>
@@ -1267,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32" s="6" t="n">
         <v>75.60000000000001</v>
       </c>
@@ -1290,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:11">
       <c r="A33" s="6" t="n">
         <v>79.2</v>
       </c>
@@ -1313,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:11">
       <c r="A34" s="6" t="n">
         <v>82.8</v>
       </c>
@@ -1336,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:11">
       <c r="A35" s="6" t="n">
         <v>86.40000000000001</v>
       </c>
@@ -1359,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:11">
       <c r="A36" s="6" t="n">
         <v>90</v>
       </c>
@@ -1382,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" s="6" t="n">
         <v>93.60000000000001</v>
       </c>
@@ -1405,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:11">
       <c r="A38" s="6" t="n">
         <v>97.2</v>
       </c>
@@ -1428,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="A39" s="6" t="n">
         <v>100.8</v>
       </c>
@@ -1451,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:11">
       <c r="A40" s="6" t="n">
         <v>104.4</v>
       </c>
@@ -1474,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41" s="6" t="n">
         <v>108</v>
       </c>
@@ -1497,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42" s="6" t="n">
         <v>111.6</v>
       </c>
@@ -1520,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:11">
       <c r="A43" s="6" t="n">
         <v>115.2</v>
       </c>
@@ -1543,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44" s="6" t="n">
         <v>118.8</v>
       </c>
@@ -1566,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45" s="6" t="n">
         <v>122.4</v>
       </c>
@@ -1589,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:11">
       <c r="A46" s="6" t="n">
         <v>126</v>
       </c>
@@ -1612,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:11">
       <c r="A47" s="6" t="n">
         <v>129.6</v>
       </c>
@@ -1635,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48" s="6" t="n">
         <v>133.2</v>
       </c>
@@ -1658,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:11">
       <c r="A49" s="6" t="n">
         <v>136.8</v>
       </c>
@@ -1681,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:11">
       <c r="A50" s="6" t="n">
         <v>140.4</v>
       </c>
@@ -1704,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:11">
       <c r="A51" s="6" t="n">
         <v>144</v>
       </c>
@@ -1727,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:11">
       <c r="A52" s="6" t="n">
         <v>147.6</v>
       </c>
@@ -1750,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:11">
       <c r="A53" s="6" t="n">
         <v>151.2</v>
       </c>
@@ -1773,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:11">
       <c r="A54" s="6" t="n">
         <v>154.8</v>
       </c>
@@ -1796,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:11">
       <c r="A55" s="6" t="n">
         <v>158.4</v>
       </c>
@@ -1819,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:11">
       <c r="A56" s="6" t="n">
         <v>162</v>
       </c>
@@ -1842,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:11">
       <c r="A57" s="6" t="n">
         <v>165.6</v>
       </c>
@@ -1865,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:11">
       <c r="A58" s="6" t="n">
         <v>169.2</v>
       </c>
@@ -1888,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:11">
       <c r="A59" s="6" t="n">
         <v>172.8</v>
       </c>
@@ -1911,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:11">
       <c r="A60" s="6" t="n">
         <v>176.4</v>
       </c>
@@ -1934,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:11">
       <c r="A61" s="6" t="n">
         <v>180</v>
       </c>
@@ -1957,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:11">
       <c r="A62" s="6" t="n">
         <v>183.6</v>
       </c>
@@ -1980,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:11">
       <c r="A63" s="6" t="n">
         <v>187.2</v>
       </c>
@@ -2003,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:11">
       <c r="A64" s="6" t="n">
         <v>190.8</v>
       </c>
@@ -2026,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:11">
       <c r="A65" s="6" t="n">
         <v>194.4</v>
       </c>
@@ -2049,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:11">
       <c r="A66" s="6" t="n">
         <v>198</v>
       </c>
@@ -2072,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:11">
       <c r="A67" s="6" t="n">
         <v>201.6</v>
       </c>
@@ -2095,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:11">
       <c r="A68" s="6" t="n">
         <v>205.2</v>
       </c>
@@ -2118,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:11">
       <c r="A69" s="6" t="n">
         <v>208.8</v>
       </c>
@@ -2141,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:11">
       <c r="A70" s="6" t="n">
         <v>212.4</v>
       </c>
@@ -2164,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:11">
       <c r="A71" s="6" t="n">
         <v>216</v>
       </c>
@@ -2187,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:11">
       <c r="A72" s="6" t="n">
         <v>219.6</v>
       </c>
@@ -2210,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:11">
       <c r="A73" s="6" t="n">
         <v>223.2</v>
       </c>
@@ -2233,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:11">
       <c r="A74" s="6" t="n">
         <v>226.8</v>
       </c>
@@ -2256,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:11">
       <c r="A75" s="6" t="n">
         <v>230.4</v>
       </c>
@@ -2279,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:11">
       <c r="A76" s="6" t="n">
         <v>234</v>
       </c>
@@ -2302,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:11">
       <c r="A77" s="6" t="n">
         <v>237.6</v>
       </c>
@@ -2325,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:11">
       <c r="A78" s="6" t="n">
         <v>241.2</v>
       </c>
@@ -2348,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:11">
       <c r="A79" s="6" t="n">
         <v>244.8</v>
       </c>
@@ -2371,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:11">
       <c r="A80" s="6" t="n">
         <v>248.4</v>
       </c>
@@ -2394,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:11">
       <c r="A81" s="6" t="n">
         <v>252</v>
       </c>
@@ -2417,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:11">
       <c r="A82" s="6" t="n">
         <v>255.6</v>
       </c>
@@ -2440,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:11">
       <c r="A83" s="6" t="n">
         <v>259.2</v>
       </c>
@@ -2463,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:11">
       <c r="A84" s="6" t="n">
         <v>262.8</v>
       </c>
@@ -2486,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:11">
       <c r="A85" s="6" t="n">
         <v>266.4</v>
       </c>
@@ -2509,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:11">
       <c r="A86" s="6" t="n">
         <v>270</v>
       </c>
@@ -2532,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:11">
       <c r="A87" s="6" t="n">
         <v>273.6</v>
       </c>
@@ -2555,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:11">
       <c r="A88" s="6" t="n">
         <v>277.2</v>
       </c>
@@ -2578,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:11">
       <c r="A89" s="6" t="n">
         <v>280.8</v>
       </c>
@@ -2601,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:11">
       <c r="A90" s="6" t="n">
         <v>284.4</v>
       </c>
@@ -2624,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:11">
       <c r="A91" s="6" t="n">
         <v>288</v>
       </c>
@@ -2647,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:11">
       <c r="A92" s="6" t="n">
         <v>291.6</v>
       </c>
@@ -2670,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:11">
       <c r="A93" s="6" t="n">
         <v>295.2</v>
       </c>
@@ -2693,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:11">
       <c r="A94" s="6" t="n">
         <v>298.8</v>
       </c>
@@ -2716,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:11">
       <c r="A95" s="6" t="n">
         <v>302.4</v>
       </c>
@@ -2739,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:11">
       <c r="A96" s="6" t="n">
         <v>306</v>
       </c>
@@ -2762,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:11">
       <c r="A97" s="6" t="n">
         <v>309.6</v>
       </c>
@@ -2785,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:11">
       <c r="A98" s="6" t="n">
         <v>313.2</v>
       </c>
@@ -2808,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:11">
       <c r="A99" s="6" t="n">
         <v>316.8</v>
       </c>
@@ -2831,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:11">
       <c r="A100" s="6" t="n">
         <v>320.4</v>
       </c>
@@ -2854,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:11">
       <c r="A101" s="6" t="n">
         <v>324</v>
       </c>
@@ -2877,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:11">
       <c r="A102" s="6" t="n">
         <v>327.6</v>
       </c>
@@ -2900,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:11">
       <c r="A103" s="6" t="n">
         <v>331.2</v>
       </c>
@@ -2923,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:11">
       <c r="A104" s="6" t="n">
         <v>334.8</v>
       </c>
@@ -2946,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:11">
       <c r="A105" s="6" t="n">
         <v>338.4</v>
       </c>
@@ -2969,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:11">
       <c r="A106" s="6" t="n">
         <v>342</v>
       </c>
@@ -2992,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:11">
       <c r="A107" s="6" t="n">
         <v>345.6</v>
       </c>
@@ -3015,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:11">
       <c r="A108" s="6" t="n">
         <v>349.2</v>
       </c>
@@ -3038,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:11">
       <c r="A109" s="6" t="n">
         <v>352.8</v>
       </c>
@@ -3061,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:11">
       <c r="A110" s="6" t="n">
         <v>356.4</v>
       </c>
@@ -3084,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:11">
       <c r="A111" s="6" t="n">
         <v>360</v>
       </c>

</xml_diff>

<commit_message>
improved readability of function names, fixed report bug
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Gain Testing Report</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>DUT Serial Number:</t>
+  </si>
+  <si>
+    <t>dfghgh</t>
   </si>
   <si>
     <t>Tested By:</t>
@@ -607,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>42928</v>
+        <v>42929</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -624,50 +627,52 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s"/>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s"/>
       <c r="B7" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="6" t="n">
         <v>100000000</v>
@@ -675,7 +680,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6">
         <f>MAX(B11:B111)</f>
@@ -702,7 +707,7 @@
         <v/>
       </c>
       <c r="I8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" s="6" t="n">
         <v>200000</v>
@@ -710,7 +715,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6">
         <f>AVERAGE(B11:B111)</f>
@@ -737,7 +742,7 @@
         <v/>
       </c>
       <c r="I9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>3</v>
@@ -745,28 +750,28 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J10" s="6" t="n">
         <v>0.025</v>
@@ -795,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -821,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J12" s="6" t="n">
         <v>0</v>
@@ -850,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J13" s="6" t="n">
         <v>0</v>
@@ -879,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J14" s="6" t="n">
         <v>0</v>
@@ -908,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>0</v>
@@ -937,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J16" s="6" t="n">
         <v>-21.99020831627661</v>
@@ -966,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J17" s="6" t="n">
         <v>0</v>
@@ -995,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J18" s="6" t="n">
         <v>0</v>
@@ -1024,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J19" s="6" t="n">
         <v>-21.99020831627661</v>

</xml_diff>

<commit_message>
Added reverse compatability for HP specan, added some annotation
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Gain Testing Report</t>
   </si>
@@ -25,6 +25,9 @@
     <t>DUT Label:</t>
   </si>
   <si>
+    <t>sdfds</t>
+  </si>
+  <si>
     <t>Customer:</t>
   </si>
   <si>
@@ -34,12 +37,21 @@
     <t>DUT Serial Number:</t>
   </si>
   <si>
+    <t>sdfdsf</t>
+  </si>
+  <si>
     <t>Tested By:</t>
   </si>
   <si>
+    <t>sdfsdsdff</t>
+  </si>
+  <si>
     <t>Comments:</t>
   </si>
   <si>
+    <t>sdf</t>
+  </si>
+  <si>
     <t>Test Data</t>
   </si>
   <si>
@@ -110,6 +122,9 @@
   </si>
   <si>
     <t>Rx Cable Loss (dB):</t>
+  </si>
+  <si>
+    <t>fgf(dB):</t>
   </si>
   <si>
     <t>Total (dB):</t>
@@ -268,7 +283,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="17487900" cy="8553450"/>
+    <ext cx="12211050" cy="5581650"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="2" name="Image 2"/>
@@ -607,75 +622,83 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>42933</v>
+        <v>42941</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s"/>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s"/>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s"/>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s"/>
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s"/>
       <c r="B7" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1000000000</v>
+        <v>2450000000</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6">
         <f>MAX(B11:B111)</f>
@@ -702,7 +725,7 @@
         <v/>
       </c>
       <c r="I8" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J8" s="6" t="n">
         <v>200000</v>
@@ -710,7 +733,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6">
         <f>AVERAGE(B11:B111)</f>
@@ -737,7 +760,7 @@
         <v/>
       </c>
       <c r="I9" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>3</v>
@@ -745,28 +768,28 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J10" s="6" t="n">
         <v>0.025</v>
@@ -795,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -821,10 +844,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J12" s="6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -850,10 +873,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>0</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -879,10 +902,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>0</v>
+        <v>-7.037752032</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -908,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>0</v>
@@ -937,10 +960,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J16" s="6" t="n">
-        <v>-41.99020831627661</v>
+        <v>-49.77353000356726</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -966,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J17" s="6" t="n">
         <v>0</v>
@@ -995,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J18" s="6" t="n">
         <v>0</v>
@@ -1024,10 +1047,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J19" s="6" t="n">
-        <v>-41.99020831627661</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1051,6 +1074,12 @@
       </c>
       <c r="G20" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="6" t="n">
+        <v>-11.56128203556726</v>
       </c>
     </row>
     <row r="21" spans="1:11">

</xml_diff>

<commit_message>
Completed EMC testing, started EMC automatic reporting
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -6,7 +6,10 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Overview &amp; Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Plots" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="EMC Compliance" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Gain Testing Report</t>
   </si>
@@ -25,9 +28,6 @@
     <t>DUT Label:</t>
   </si>
   <si>
-    <t>sdfds</t>
-  </si>
-  <si>
     <t>Customer:</t>
   </si>
   <si>
@@ -37,21 +37,12 @@
     <t>DUT Serial Number:</t>
   </si>
   <si>
-    <t>sdfdsf</t>
-  </si>
-  <si>
     <t>Tested By:</t>
   </si>
   <si>
-    <t>sdfsdsdff</t>
-  </si>
-  <si>
     <t>Comments:</t>
   </si>
   <si>
-    <t>sdf</t>
-  </si>
-  <si>
     <t>Test Data</t>
   </si>
   <si>
@@ -124,10 +115,28 @@
     <t>Rx Cable Loss (dB):</t>
   </si>
   <si>
-    <t>fgf(dB):</t>
-  </si>
-  <si>
     <t>Total (dB):</t>
+  </si>
+  <si>
+    <t>Data Collection Plots</t>
+  </si>
+  <si>
+    <t>EMC Compliance Testing Result</t>
+  </si>
+  <si>
+    <t>Regulator:</t>
+  </si>
+  <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>Class:</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Electric Field Limit (dBuV/m):</t>
   </si>
 </sst>
 </file>
@@ -276,14 +285,99 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>10</col>
+      <col>5</col>
       <colOff>0</colOff>
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="12211050" cy="5581650"/>
+    <ext cx="1619250" cy="942975"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="13982700" cy="6838950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="2" name="Image 2"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="942975"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="2" name="Image 2"/>
@@ -593,7 +687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,93 +706,85 @@
     <col customWidth="1" max="10" min="10" width="20"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50" r="1" spans="1:11">
+    <row customHeight="1" ht="50" r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>42941</v>
+        <v>42942</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="2" t="s">
+      <c r="B5" t="s"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="I6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" s="4" t="s"/>
       <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="J7" s="6" t="n">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>2450000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="B8" s="6">
         <f>MAX(B11:B111)</f>
@@ -725,15 +811,15 @@
         <v/>
       </c>
       <c r="I8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J8" s="6" t="n">
         <v>200000</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6">
         <f>AVERAGE(B11:B111)</f>
@@ -760,42 +846,42 @@
         <v/>
       </c>
       <c r="I9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J10" s="6" t="n">
         <v>0.025</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:10">
       <c r="A11" s="6" t="n">
         <v>0</v>
       </c>
@@ -818,10 +904,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="6" t="n">
         <v>3.6</v>
       </c>
@@ -844,13 +930,13 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J12" s="6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="n">
         <v>7.2</v>
       </c>
@@ -873,13 +959,13 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>33.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="6" t="n">
         <v>10.8</v>
       </c>
@@ -902,13 +988,13 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>-7.037752032</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="6" t="n">
         <v>14.4</v>
       </c>
@@ -931,13 +1017,13 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:10">
       <c r="A16" s="6" t="n">
         <v>18</v>
       </c>
@@ -960,13 +1046,13 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J16" s="6" t="n">
-        <v>-49.77353000356726</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>-21.99020831627661</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="6" t="n">
         <v>21.6</v>
       </c>
@@ -989,13 +1075,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J17" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:10">
       <c r="A18" s="6" t="n">
         <v>25.2</v>
       </c>
@@ -1018,13 +1104,13 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J18" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:10">
       <c r="A19" s="6" t="n">
         <v>28.8</v>
       </c>
@@ -1047,13 +1133,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J19" s="6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>-21.99020831627661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="6" t="n">
         <v>32.4</v>
       </c>
@@ -1075,14 +1161,8 @@
       <c r="G20" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="6" t="n">
-        <v>-11.56128203556726</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="6" t="n">
         <v>36</v>
       </c>
@@ -1105,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:10">
       <c r="A22" s="6" t="n">
         <v>39.6</v>
       </c>
@@ -1128,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:10">
       <c r="A23" s="6" t="n">
         <v>43.2</v>
       </c>
@@ -1151,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:10">
       <c r="A24" s="6" t="n">
         <v>46.8</v>
       </c>
@@ -1174,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:10">
       <c r="A25" s="6" t="n">
         <v>50.4</v>
       </c>
@@ -1197,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:10">
       <c r="A26" s="6" t="n">
         <v>54</v>
       </c>
@@ -1220,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:10">
       <c r="A27" s="6" t="n">
         <v>57.6</v>
       </c>
@@ -1243,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:10">
       <c r="A28" s="6" t="n">
         <v>61.2</v>
       </c>
@@ -1266,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:10">
       <c r="A29" s="6" t="n">
         <v>64.8</v>
       </c>
@@ -1289,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:10">
       <c r="A30" s="6" t="n">
         <v>68.40000000000001</v>
       </c>
@@ -1312,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:10">
       <c r="A31" s="6" t="n">
         <v>72</v>
       </c>
@@ -1335,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:10">
       <c r="A32" s="6" t="n">
         <v>75.60000000000001</v>
       </c>
@@ -1358,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:10">
       <c r="A33" s="6" t="n">
         <v>79.2</v>
       </c>
@@ -1381,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:10">
       <c r="A34" s="6" t="n">
         <v>82.8</v>
       </c>
@@ -1404,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:10">
       <c r="A35" s="6" t="n">
         <v>86.40000000000001</v>
       </c>
@@ -1427,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:10">
       <c r="A36" s="6" t="n">
         <v>90</v>
       </c>
@@ -1450,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:10">
       <c r="A37" s="6" t="n">
         <v>93.60000000000001</v>
       </c>
@@ -1473,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:10">
       <c r="A38" s="6" t="n">
         <v>97.2</v>
       </c>
@@ -1496,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:10">
       <c r="A39" s="6" t="n">
         <v>100.8</v>
       </c>
@@ -1519,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:10">
       <c r="A40" s="6" t="n">
         <v>104.4</v>
       </c>
@@ -1542,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:10">
       <c r="A41" s="6" t="n">
         <v>108</v>
       </c>
@@ -1565,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:10">
       <c r="A42" s="6" t="n">
         <v>111.6</v>
       </c>
@@ -1588,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:10">
       <c r="A43" s="6" t="n">
         <v>115.2</v>
       </c>
@@ -1611,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:10">
       <c r="A44" s="6" t="n">
         <v>118.8</v>
       </c>
@@ -1634,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:10">
       <c r="A45" s="6" t="n">
         <v>122.4</v>
       </c>
@@ -1657,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:10">
       <c r="A46" s="6" t="n">
         <v>126</v>
       </c>
@@ -1680,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:10">
       <c r="A47" s="6" t="n">
         <v>129.6</v>
       </c>
@@ -1703,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:10">
       <c r="A48" s="6" t="n">
         <v>133.2</v>
       </c>
@@ -1726,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:10">
       <c r="A49" s="6" t="n">
         <v>136.8</v>
       </c>
@@ -1749,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:10">
       <c r="A50" s="6" t="n">
         <v>140.4</v>
       </c>
@@ -1772,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:10">
       <c r="A51" s="6" t="n">
         <v>144</v>
       </c>
@@ -1795,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:10">
       <c r="A52" s="6" t="n">
         <v>147.6</v>
       </c>
@@ -1818,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:10">
       <c r="A53" s="6" t="n">
         <v>151.2</v>
       </c>
@@ -1841,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:10">
       <c r="A54" s="6" t="n">
         <v>154.8</v>
       </c>
@@ -1864,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:10">
       <c r="A55" s="6" t="n">
         <v>158.4</v>
       </c>
@@ -1887,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:10">
       <c r="A56" s="6" t="n">
         <v>162</v>
       </c>
@@ -1910,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:10">
       <c r="A57" s="6" t="n">
         <v>165.6</v>
       </c>
@@ -1933,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:10">
       <c r="A58" s="6" t="n">
         <v>169.2</v>
       </c>
@@ -1956,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:10">
       <c r="A59" s="6" t="n">
         <v>172.8</v>
       </c>
@@ -1979,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:10">
       <c r="A60" s="6" t="n">
         <v>176.4</v>
       </c>
@@ -2002,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:10">
       <c r="A61" s="6" t="n">
         <v>180</v>
       </c>
@@ -2025,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:10">
       <c r="A62" s="6" t="n">
         <v>183.6</v>
       </c>
@@ -2048,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:10">
       <c r="A63" s="6" t="n">
         <v>187.2</v>
       </c>
@@ -2071,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:10">
       <c r="A64" s="6" t="n">
         <v>190.8</v>
       </c>
@@ -2094,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:10">
       <c r="A65" s="6" t="n">
         <v>194.4</v>
       </c>
@@ -2117,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:10">
       <c r="A66" s="6" t="n">
         <v>198</v>
       </c>
@@ -2140,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:10">
       <c r="A67" s="6" t="n">
         <v>201.6</v>
       </c>
@@ -2163,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:10">
       <c r="A68" s="6" t="n">
         <v>205.2</v>
       </c>
@@ -2186,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:10">
       <c r="A69" s="6" t="n">
         <v>208.8</v>
       </c>
@@ -2209,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:10">
       <c r="A70" s="6" t="n">
         <v>212.4</v>
       </c>
@@ -2232,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:10">
       <c r="A71" s="6" t="n">
         <v>216</v>
       </c>
@@ -2255,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:10">
       <c r="A72" s="6" t="n">
         <v>219.6</v>
       </c>
@@ -2278,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:10">
       <c r="A73" s="6" t="n">
         <v>223.2</v>
       </c>
@@ -2301,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:10">
       <c r="A74" s="6" t="n">
         <v>226.8</v>
       </c>
@@ -2324,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:10">
       <c r="A75" s="6" t="n">
         <v>230.4</v>
       </c>
@@ -2347,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:10">
       <c r="A76" s="6" t="n">
         <v>234</v>
       </c>
@@ -2370,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:10">
       <c r="A77" s="6" t="n">
         <v>237.6</v>
       </c>
@@ -2393,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:10">
       <c r="A78" s="6" t="n">
         <v>241.2</v>
       </c>
@@ -2416,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:10">
       <c r="A79" s="6" t="n">
         <v>244.8</v>
       </c>
@@ -2439,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:10">
       <c r="A80" s="6" t="n">
         <v>248.4</v>
       </c>
@@ -2462,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:10">
       <c r="A81" s="6" t="n">
         <v>252</v>
       </c>
@@ -2485,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:10">
       <c r="A82" s="6" t="n">
         <v>255.6</v>
       </c>
@@ -2508,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:10">
       <c r="A83" s="6" t="n">
         <v>259.2</v>
       </c>
@@ -2531,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:10">
       <c r="A84" s="6" t="n">
         <v>262.8</v>
       </c>
@@ -2554,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:10">
       <c r="A85" s="6" t="n">
         <v>266.4</v>
       </c>
@@ -2577,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:10">
       <c r="A86" s="6" t="n">
         <v>270</v>
       </c>
@@ -2600,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:10">
       <c r="A87" s="6" t="n">
         <v>273.6</v>
       </c>
@@ -2623,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:10">
       <c r="A88" s="6" t="n">
         <v>277.2</v>
       </c>
@@ -2646,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:10">
       <c r="A89" s="6" t="n">
         <v>280.8</v>
       </c>
@@ -2669,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:10">
       <c r="A90" s="6" t="n">
         <v>284.4</v>
       </c>
@@ -2692,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:10">
       <c r="A91" s="6" t="n">
         <v>288</v>
       </c>
@@ -2715,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:10">
       <c r="A92" s="6" t="n">
         <v>291.6</v>
       </c>
@@ -2738,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:10">
       <c r="A93" s="6" t="n">
         <v>295.2</v>
       </c>
@@ -2761,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:10">
       <c r="A94" s="6" t="n">
         <v>298.8</v>
       </c>
@@ -2784,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:10">
       <c r="A95" s="6" t="n">
         <v>302.4</v>
       </c>
@@ -2807,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:10">
       <c r="A96" s="6" t="n">
         <v>306</v>
       </c>
@@ -2830,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:10">
       <c r="A97" s="6" t="n">
         <v>309.6</v>
       </c>
@@ -2853,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:10">
       <c r="A98" s="6" t="n">
         <v>313.2</v>
       </c>
@@ -2876,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:10">
       <c r="A99" s="6" t="n">
         <v>316.8</v>
       </c>
@@ -2899,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:10">
       <c r="A100" s="6" t="n">
         <v>320.4</v>
       </c>
@@ -2922,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:10">
       <c r="A101" s="6" t="n">
         <v>324</v>
       </c>
@@ -2945,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:10">
       <c r="A102" s="6" t="n">
         <v>327.6</v>
       </c>
@@ -2968,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:10">
       <c r="A103" s="6" t="n">
         <v>331.2</v>
       </c>
@@ -2991,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:10">
       <c r="A104" s="6" t="n">
         <v>334.8</v>
       </c>
@@ -3014,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:10">
       <c r="A105" s="6" t="n">
         <v>338.4</v>
       </c>
@@ -3037,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:10">
       <c r="A106" s="6" t="n">
         <v>342</v>
       </c>
@@ -3060,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:10">
       <c r="A107" s="6" t="n">
         <v>345.6</v>
       </c>
@@ -3083,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:10">
       <c r="A108" s="6" t="n">
         <v>349.2</v>
       </c>
@@ -3106,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:10">
       <c r="A109" s="6" t="n">
         <v>352.8</v>
       </c>
@@ -3129,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:10">
       <c r="A110" s="6" t="n">
         <v>356.4</v>
       </c>
@@ -3152,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:10">
       <c r="A111" s="6" t="n">
         <v>360</v>
       </c>
@@ -3185,4 +3265,118 @@
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="20"/>
+    <col customWidth="1" max="2" min="2" width="20"/>
+    <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="50" r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="30"/>
+    <col customWidth="1" max="2" min="2" width="20"/>
+    <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="50" r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed 3d rendering and added it to application
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Gain Testing Report</t>
   </si>
@@ -124,7 +124,7 @@
     <t>EMC Compliance Testing Result</t>
   </si>
   <si>
-    <t>Regulator:</t>
+    <t>Regulatory Convention:</t>
   </si>
   <si>
     <t>FCC</t>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Electric Field Limit (dBuV/m):</t>
+  </si>
+  <si>
+    <t>Test Status:</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Error Margin (dB):</t>
   </si>
 </sst>
 </file>
@@ -322,7 +331,7 @@
       <row>3</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="13982700" cy="6838950"/>
+    <ext cx="13115925" cy="6410325"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="2" name="Image 2"/>
@@ -377,7 +386,7 @@
       <row>9</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6096000" cy="4572000"/>
+    <ext cx="7620000" cy="5715000"/>
     <pic>
       <nvPicPr>
         <cNvPr descr="Picture" id="2" name="Image 2"/>
@@ -716,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>42942</v>
+        <v>42947</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -3353,6 +3362,22 @@
         <v>43.5</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="10" spans="1:4"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>